<commit_message>
Rewrote the SkillSearch to work for any character. Pulls skill multiplier values for specified character and skill type.
</commit_message>
<xml_diff>
--- a/DataTables/Characters/IttoTables.xlsx
+++ b/DataTables/Characters/IttoTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GenshinCode\GenshinIndex\DataTables\Characters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2BD19A-F8F3-4B92-A275-D35A3565A5C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA258E8-87B9-4E1C-A736-0D41ED0BAFE8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="2160" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="285" yWindow="5175" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="6" r:id="rId1"/>
@@ -1065,7 +1065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EA1C57-3921-476D-A8D1-199BC3F3FCFE}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -1386,8 +1386,8 @@
   </sheetPr>
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
The imports are scuffed as fuck. Need to either restructure the entire project in a way that packages are nested within each other. Or figure out how to call modules from other packages. It seems the PYTHONPATH is somehow off and it can't locate the packages even when I use the right syntax. This might be a problem just with Visual Studio Code, so it might be worth testing in Pycharm, but this might take some extra steps to solve completely, especially in VS code.
</commit_message>
<xml_diff>
--- a/DataTables/Characters/IttoTables.xlsx
+++ b/DataTables/Characters/IttoTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GenshinCode\GenshinIndex\DataTables\Characters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA258E8-87B9-4E1C-A736-0D41ED0BAFE8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD0C715-B7D1-4285-B38F-55543D7E4C45}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="5175" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="7605" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="6" r:id="rId1"/>
@@ -1387,7 +1387,7 @@
   <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>